<commit_message>
Added Scrum report, Sprint backlog
</commit_message>
<xml_diff>
--- a/docs/Getana_Deliverable_2_ProductBacklog.xlsx
+++ b/docs/Getana_Deliverable_2_ProductBacklog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshyam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -702,37 +702,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="69.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="69.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="1025" width="11.5546875"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -752,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -760,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -772,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -780,7 +780,7 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -792,7 +792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -800,7 +800,7 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -812,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -820,7 +820,7 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
@@ -832,7 +832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>8</v>
       </c>
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>9</v>
       </c>
@@ -872,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>15</v>
       </c>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>21</v>
       </c>
@@ -912,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>10</v>
       </c>
@@ -932,7 +932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>11</v>
       </c>
@@ -952,7 +952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>12</v>
       </c>
@@ -972,7 +972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>4</v>
       </c>
@@ -992,7 +992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>16</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>17</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>14</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>7</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>20</v>
       </c>
@@ -1172,19 +1172,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B33" s="5" t="s">
         <v>52</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B34" s="5" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
created a create schedule screen, will add some user stories from focus goup in a while
</commit_message>
<xml_diff>
--- a/docs/Getana_Deliverable_2_ProductBacklog.xlsx
+++ b/docs/Getana_Deliverable_2_ProductBacklog.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshyam\Downloads\Raidernav\RaiderNAV\docs\deliverable 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sakshyam\Downloads\Raidernav\RaiderNAV\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D2732E-B355-4617-951B-3E8B32305BC3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1445,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9A065E-4731-4DE3-908D-A57CA57C4E88}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1573,58 +1574,58 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>21</v>
+        <v>52</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="F13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>21</v>
@@ -1633,118 +1634,118 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
       <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18">
+      <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19">
         <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>21</v>
@@ -1755,142 +1756,142 @@
     </row>
     <row r="21" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22">
+      <c r="E23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="66" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:7" ht="66" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>17</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23">
+      <c r="E24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24">
         <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>14</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>6</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="27" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>13</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>11</v>
+      <c r="E27" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">

</xml_diff>